<commit_message>
update tai chinh sau ky hop dong thue nha
</commit_message>
<xml_diff>
--- a/WIP/Documents/X-Life_TaiChinh.xlsx
+++ b/WIP/Documents/X-Life_TaiChinh.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>STT</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t>Đặt cọc thuê văn phòng cho anh Vỹ</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Vốn đã góp</t>
+  </si>
+  <si>
+    <t>HaiPM</t>
+  </si>
+  <si>
+    <t>DaoHVN</t>
+  </si>
+  <si>
+    <t>MinhTT</t>
+  </si>
+  <si>
+    <t>TrungHV</t>
+  </si>
+  <si>
+    <t>Ký hợp đồng thuê 6 tháng</t>
   </si>
 </sst>
 </file>
@@ -55,9 +76,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,6 +97,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,10 +135,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -133,8 +163,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E7" totalsRowCount="1">
-  <autoFilter ref="A3:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:E15" totalsRowCount="1">
+  <autoFilter ref="A8:E14"/>
   <tableColumns count="5">
     <tableColumn id="1" name="STT" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Ngày"/>
@@ -468,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -482,59 +512,128 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>55500000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2">
-        <f>SUM(Table1[Thu])-SUM(Table1[Chi])</f>
-        <v>-8500000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D6" s="2">
+        <f>SUM(D2:D5)- SUM(Table1[Thu])-SUM(Table1[Chi])</f>
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B9" s="1">
         <v>42454</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D9" s="2">
         <v>8500000</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42458</v>
+      </c>
+      <c r="D10" s="2">
+        <v>51000000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C15">
         <f>SUBTOTAL(109,Table1[Thu])</f>
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D15">
         <f>SUBTOTAL(109,Table1[Chi])</f>
-        <v>8500000</v>
-      </c>
-      <c r="E7">
+        <v>59500000</v>
+      </c>
+      <c r="E15">
         <f>SUBTOTAL(103,Table1[Chi tiết])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tai chinh 0426
update tai chinh 0426
</commit_message>
<xml_diff>
--- a/WIP/Documents/X-Life_TaiChinh.xlsx
+++ b/WIP/Documents/X-Life_TaiChinh.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="193">
   <si>
     <t>STT</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Mặt bằng</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>Bổ sung 20m dây loa</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t>Sofa</t>
   </si>
   <si>
-    <t>Kính cường lực</t>
-  </si>
-  <si>
     <t>Nhân viên kinh doanh phần mềm kế toán (Nam Việt Luật)
 Thiết kế giao diện website (Thiết Long)
 Làm offer cho phần mềm điện thoại smart phone
@@ -479,9 +473,6 @@
     <t>4 đèn trần cho phòng ngủ</t>
   </si>
   <si>
-    <t>sơn maxilite 1t</t>
-  </si>
-  <si>
     <t>bột tít expo</t>
   </si>
   <si>
@@ -630,9 +621,6 @@
     <t>Khác</t>
   </si>
   <si>
-    <t>Phí mua hàng chưa trả</t>
-  </si>
-  <si>
     <t>Số dư X-Life thực</t>
   </si>
   <si>
@@ -640,6 +628,87 @@
   </si>
   <si>
     <t>Số dư X-Life(tiền mặt)</t>
+  </si>
+  <si>
+    <t>Quảng cáo</t>
+  </si>
+  <si>
+    <t>Tờ rơi</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Thanh toán cửa kính</t>
+  </si>
+  <si>
+    <t>Tất toán sofa(đã đồng ý làm thêm kê)</t>
+  </si>
+  <si>
+    <t>Đầu tư</t>
+  </si>
+  <si>
+    <t>Thiết bị nghiên cứu</t>
+  </si>
+  <si>
+    <t>Board để phát triển hệ thống</t>
+  </si>
+  <si>
+    <t>Đồ cúng khai trương</t>
+  </si>
+  <si>
+    <t>sơn maxilite 1l</t>
+  </si>
+  <si>
+    <t>2 thùng sơn expo (sơn lại tường)</t>
+  </si>
+  <si>
+    <t>NameCard</t>
+  </si>
+  <si>
+    <t>NameCard cho 3 member</t>
+  </si>
+  <si>
+    <t>Nẹp chỉ điện</t>
+  </si>
+  <si>
+    <t>Logo SMH BKAV</t>
+  </si>
+  <si>
+    <t>Đèn ngủ</t>
+  </si>
+  <si>
+    <t>mua 11m dây 1.5+ 2 nẹp 3F+ 1 hộp đinh</t>
+  </si>
+  <si>
+    <t>mua 1mũi khoan+ 3 cây ti pi6+ ticke nhựa 2 túi+</t>
+  </si>
+  <si>
+    <t>Phí mua hàng chưa trả/dự chi</t>
+  </si>
+  <si>
+    <t>Đặt cọc bộ drap giường</t>
+  </si>
+  <si>
+    <t>drap giường</t>
+  </si>
+  <si>
+    <t>đèn tranh</t>
+  </si>
+  <si>
+    <t>đi lại điều hòa</t>
+  </si>
+  <si>
+    <t>Đặt cọc kệ tivi + Bàn lễ tân + Đôn đèn ngủ</t>
+  </si>
+  <si>
+    <t>kệ tivi + Bàn lễ tân + Đôn đèn ngủ</t>
+  </si>
+  <si>
+    <t>Tranh tường</t>
+  </si>
+  <si>
+    <t>Rèm cuốn + động cơ</t>
   </si>
 </sst>
 </file>
@@ -845,8 +914,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:H44" totalsRowCount="1">
-  <autoFilter ref="A10:H43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:H63" totalsRowCount="1">
+  <autoFilter ref="A10:H62"/>
   <tableColumns count="8">
     <tableColumn id="1" name="STT" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Ngày" dataDxfId="6"/>
@@ -1183,10 +1252,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F9"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="G9" activeCellId="1" sqref="C1:G9 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1211,19 +1283,19 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="K1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1231,21 +1303,21 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <f>4000000+10000000+10000000</f>
-        <v>24000000</v>
+        <f>4000000+10000000+10000000+1050000+18000000</f>
+        <v>43050000</v>
       </c>
       <c r="E2" s="2">
         <f>50000000-D2</f>
-        <v>26000000</v>
+        <v>6950000</v>
       </c>
       <c r="F2" s="2">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K2" s="2">
         <f>Budget!E2</f>
@@ -1265,20 +1337,21 @@
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <v>55500000</v>
+        <f>55500000+20000000+24500000</f>
+        <v>100000000</v>
       </c>
       <c r="E3" s="2">
         <f>100000000-D3</f>
-        <v>44500000</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K3" s="2">
         <f>Budget!E3</f>
@@ -1286,11 +1359,11 @@
       </c>
       <c r="L3" s="2">
         <f>SUMIFS(Table1[Chi],Table1[Phân loại],"Thiết bị") + SUMIFS(Table1[Chi],Table1[Phân loại],"Mặt bằng")</f>
-        <v>28146000</v>
+        <v>110841625</v>
       </c>
       <c r="M3" s="2">
         <f>K3-L3</f>
-        <v>148974000</v>
+        <v>66278375</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1304,9 +1377,14 @@
         <f>50000000-D4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>500000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>188</v>
+      </c>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K4" s="2">
         <f>Budget!E4</f>
@@ -1322,22 +1400,27 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>3600000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>190</v>
+      </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2">
         <f>SUM(Table1[Chi])-SUM(L2:L4)</f>
-        <v>1506000</v>
+        <v>3948000</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1346,37 +1429,38 @@
       </c>
       <c r="D6" s="21">
         <f>SUM(D2:D5)</f>
-        <v>129500000</v>
-      </c>
-      <c r="E6" s="21">
-        <f>SUM(E2:E5)</f>
-        <v>70500000</v>
+        <v>193050000</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(F2:F5)</f>
-        <v>20000000</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>1500000</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D7" s="21">
         <f>SUM(D2:D5)+SUM(Table1[Thu])-SUM(Table1[Chi])</f>
-        <v>40348000</v>
+        <v>18760375</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>6000000</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D8" s="22">
-        <f>D7-F6</f>
-        <v>20348000</v>
+        <f>D7-F9</f>
+        <v>4360375</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1384,11 +1468,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" s="23" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D9" s="24">
-        <f>D8+E6</f>
-        <v>90848000</v>
+        <f>D8+E9</f>
+        <v>11310375</v>
+      </c>
+      <c r="E9" s="21">
+        <f>SUM(E2:E5)</f>
+        <v>6950000</v>
+      </c>
+      <c r="F9" s="2">
+        <f>SUM(F2:F8)</f>
+        <v>14400000</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1405,10 +1497,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1428,10 +1520,10 @@
         <v>8500000</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -1452,10 +1544,10 @@
         <v>51000000</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -1476,10 +1568,10 @@
         <v>1076000</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>69</v>
+        <v>168</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
@@ -1500,10 +1592,10 @@
         <v>100000</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -1525,10 +1617,10 @@
         <v>590000</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
@@ -1549,10 +1641,10 @@
         <v>2000000</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G16" t="s">
         <v>15</v>
@@ -1573,10 +1665,10 @@
         <v>438000</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G17" t="s">
         <v>17</v>
@@ -1598,10 +1690,10 @@
         <v>1020000</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
@@ -1622,10 +1714,10 @@
         <v>280000</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
@@ -1646,10 +1738,10 @@
         <v>2000000</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" t="s">
         <v>21</v>
@@ -1673,7 +1765,7 @@
         <v>68</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
@@ -1694,10 +1786,10 @@
         <v>1000000</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G22" t="s">
         <v>63</v>
@@ -1708,7 +1800,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ref="A23:A41" si="1">A22+1</f>
+        <f t="shared" ref="A23:A57" si="1">A22+1</f>
         <v>13</v>
       </c>
       <c r="B23" s="1">
@@ -1719,10 +1811,10 @@
         <v>156000</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G23" t="s">
         <v>64</v>
@@ -1744,10 +1836,10 @@
         <v>200000</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
         <v>65</v>
@@ -1768,10 +1860,10 @@
         <v>700000</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G25" t="s">
         <v>66</v>
@@ -1795,7 +1887,7 @@
         <v>68</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
         <v>67</v>
@@ -1816,13 +1908,13 @@
         <v>140000</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H27" t="s">
         <v>11</v>
@@ -1843,10 +1935,10 @@
         <v>68</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
         <v>11</v>
@@ -1864,13 +1956,13 @@
         <v>54000</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
         <v>11</v>
@@ -1888,13 +1980,13 @@
         <v>13000</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
         <v>11</v>
@@ -1915,10 +2007,10 @@
         <v>68</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H31" t="s">
         <v>11</v>
@@ -1939,16 +2031,16 @@
         <v>68</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1963,16 +2055,16 @@
         <v>68</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1987,16 +2079,16 @@
         <v>68</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2008,19 +2100,19 @@
         <v>330000</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2032,19 +2124,19 @@
         <v>5000000</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -2059,16 +2151,16 @@
         <v>68</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2083,16 +2175,16 @@
         <v>68</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2105,19 +2197,19 @@
         <v>680000</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H39" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -2132,16 +2224,16 @@
         <v>68</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G40" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="H40" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -2156,41 +2248,433 @@
         <v>68</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B42" s="1">
+        <v>42474</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1050000</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" t="s">
+        <v>167</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B43" s="1">
+        <v>42474</v>
+      </c>
+      <c r="D43" s="7">
+        <v>15000000</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" t="s">
+        <v>169</v>
+      </c>
+      <c r="H43" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43">
+        <f>2.7+0.5+0.8+0.2+0.25+1</f>
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B44" s="1">
+        <v>42474</v>
+      </c>
+      <c r="D44" s="7">
+        <v>5000000</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G44" t="s">
+        <v>170</v>
+      </c>
+      <c r="H44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B45" s="1">
+        <v>42474</v>
+      </c>
+      <c r="D45" s="7">
+        <v>987000</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G45" t="s">
+        <v>173</v>
+      </c>
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B46" s="1">
+        <v>42474</v>
+      </c>
+      <c r="D46" s="7">
+        <v>105000</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B47" s="1">
+        <v>42475</v>
+      </c>
+      <c r="D47" s="7">
+        <v>200000</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G47" t="s">
+        <v>176</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B48" s="1">
+        <v>42479</v>
+      </c>
+      <c r="D48" s="7">
+        <v>300000</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G48" t="s">
+        <v>178</v>
+      </c>
+      <c r="H48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B49" s="1">
+        <v>42481</v>
+      </c>
+      <c r="D49" s="7">
+        <v>59805625</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G49" t="s">
+        <v>158</v>
+      </c>
+      <c r="H49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B50" s="1">
+        <v>42481</v>
+      </c>
+      <c r="D50" s="7">
+        <v>98000</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G50" t="s">
+        <v>179</v>
+      </c>
+      <c r="H50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B51" s="1">
+        <v>42482</v>
+      </c>
+      <c r="D51" s="7">
+        <v>1500000</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G51" t="s">
+        <v>189</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B52" s="1">
+        <v>42483</v>
+      </c>
+      <c r="D52" s="7">
+        <v>500000</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G52" t="s">
+        <v>185</v>
+      </c>
+      <c r="H52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B53" s="1">
+        <v>42483</v>
+      </c>
+      <c r="D53" s="7">
+        <v>200000</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G53" t="s">
+        <v>180</v>
+      </c>
+      <c r="H53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B54" s="1">
+        <v>42484</v>
+      </c>
+      <c r="D54" s="7">
+        <v>75000</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G54" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B55" s="1">
+        <v>42485</v>
+      </c>
+      <c r="D55" s="7">
+        <v>280000</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" t="s">
+        <v>181</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B56" s="1">
+        <v>42485</v>
+      </c>
+      <c r="D56" s="7">
+        <v>37000</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G56" t="s">
+        <v>183</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>5</v>
       </c>
-      <c r="C44">
+      <c r="C63">
         <f>SUBTOTAL(109,Table1[Thu])</f>
         <v>0</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D63" s="4">
         <f>SUBTOTAL(109,Table1[Chi])</f>
-        <v>89152000</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+        <v>174289625</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2221,12 +2705,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E2" s="7">
         <f>E8</f>
@@ -2239,7 +2723,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E3" s="7">
         <f>SUM(E11:E23)</f>
@@ -2250,12 +2734,12 @@
         <v>4920000</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E4" s="7">
         <f>SUM(E9:E10)</f>
@@ -2268,7 +2752,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7">
@@ -2279,7 +2763,7 @@
     </row>
     <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D6" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7">
@@ -2287,27 +2771,27 @@
         <v>97100000</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>30</v>
@@ -2318,7 +2802,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -2330,7 +2814,7 @@
         <v>7500000</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2338,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -2350,7 +2834,7 @@
         <v>3000000</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2358,7 +2842,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2370,7 +2854,7 @@
         <v>4000000</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2378,7 +2862,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2388,7 +2872,7 @@
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2397,7 +2881,7 @@
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
@@ -2412,7 +2896,7 @@
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
@@ -2427,7 +2911,7 @@
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
@@ -2442,7 +2926,7 @@
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
@@ -2450,7 +2934,7 @@
         <v>3000000</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2459,7 +2943,7 @@
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
@@ -2474,7 +2958,7 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
@@ -2482,7 +2966,7 @@
         <v>5000000</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
@@ -2491,7 +2975,7 @@
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
@@ -2499,7 +2983,7 @@
         <v>3000000</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2508,7 +2992,7 @@
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="14"/>
@@ -2516,7 +3000,7 @@
         <v>5000000</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2525,7 +3009,7 @@
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14"/>
@@ -2540,7 +3024,7 @@
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
@@ -2554,7 +3038,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -2566,7 +3050,7 @@
         <v>4800000</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,7 +3058,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -2586,7 +3070,7 @@
         <v>7200000</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2594,7 +3078,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -2752,7 +3236,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="E3" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I3">
         <v>1989</v>
@@ -2775,10 +3259,10 @@
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
@@ -2798,10 +3282,10 @@
         <v>61</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="204.75" x14ac:dyDescent="0.25">
@@ -2821,13 +3305,13 @@
         <v>4</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="189" x14ac:dyDescent="0.25">
@@ -2850,10 +3334,10 @@
         <v>54</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
@@ -2876,10 +3360,10 @@
         <v>55</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="173.25" x14ac:dyDescent="0.25">
@@ -2897,7 +3381,7 @@
         <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="236.25" x14ac:dyDescent="0.25">
@@ -2915,10 +3399,10 @@
         <v>57</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -2953,7 +3437,7 @@
         <v>58</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2994,20 +3478,20 @@
         <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F19" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F20" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tai chinh 0409
</commit_message>
<xml_diff>
--- a/WIP/Documents/X-Life_TaiChinh.xlsx
+++ b/WIP/Documents/X-Life_TaiChinh.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="205">
   <si>
     <t>STT</t>
   </si>
@@ -708,7 +708,43 @@
     <t>Tranh tường</t>
   </si>
   <si>
-    <t>Rèm cuốn + động cơ</t>
+    <t>Camera IP</t>
+  </si>
+  <si>
+    <t>tất toán drap giường</t>
+  </si>
+  <si>
+    <t>Đèn tranh</t>
+  </si>
+  <si>
+    <t>Đặt cọc rèm cuốn</t>
+  </si>
+  <si>
+    <t>Tivi + giàn loa + ampli</t>
+  </si>
+  <si>
+    <t>Tất toán kệ tivi + Bàn lễ tân + Đôn đèn ngủ</t>
+  </si>
+  <si>
+    <t>Dàn loa Sony DAV_TZ150</t>
+  </si>
+  <si>
+    <t>Smart Tivi Samsung</t>
+  </si>
+  <si>
+    <t>Tổ ong demo sản phẩm</t>
+  </si>
+  <si>
+    <t>Lương</t>
+  </si>
+  <si>
+    <t>Ứng lương tháng 5 cho Nhàn</t>
+  </si>
+  <si>
+    <t>Tổ ong show sản phẩm + phụ kiện</t>
+  </si>
+  <si>
+    <t>Ứng lương tháng 4 cho Minh</t>
   </si>
 </sst>
 </file>
@@ -914,8 +950,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:H63" totalsRowCount="1">
-  <autoFilter ref="A10:H62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A10:H73" totalsRowCount="1">
+  <autoFilter ref="A10:H72"/>
   <tableColumns count="8">
     <tableColumn id="1" name="STT" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Ngày" dataDxfId="6"/>
@@ -1252,13 +1288,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="G9" activeCellId="1" sqref="C1:G9 G9"/>
+      <selection pane="bottomRight" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1269,13 +1305,13 @@
     <col min="4" max="5" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.375" customWidth="1"/>
-    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.25" customWidth="1"/>
+    <col min="12" max="12" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>7</v>
       </c>
@@ -1288,17 +1324,17 @@
       <c r="F1" t="s">
         <v>184</v>
       </c>
+      <c r="J1" t="s">
+        <v>159</v>
+      </c>
       <c r="K1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L1" t="s">
-        <v>160</v>
-      </c>
-      <c r="M1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -1311,62 +1347,62 @@
         <v>6950000</v>
       </c>
       <c r="F2" s="2">
-        <v>2000000</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>186</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" t="s">
         <v>120</v>
       </c>
-      <c r="K2" s="2">
+      <c r="J2" s="2">
         <f>Budget!E2</f>
         <v>90000000</v>
       </c>
-      <c r="L2" s="2">
+      <c r="K2" s="2">
         <f>SUMIFS(Table1[Chi],Table1[Phân loại], "Thuê mặt bằng")</f>
         <v>59500000</v>
       </c>
-      <c r="M2" s="2">
-        <f>K2-L2</f>
+      <c r="L2" s="2">
+        <f>J2-K2</f>
         <v>30500000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <f>55500000+20000000+24500000</f>
-        <v>100000000</v>
+        <f>55500000+20000000+24500000+20000000</f>
+        <v>120000000</v>
       </c>
       <c r="E3" s="2">
-        <f>100000000-D3</f>
+        <f>150000000-D3</f>
+        <v>30000000</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>800000</v>
       </c>
       <c r="G3" t="s">
         <v>187</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" s="2">
         <f>Budget!E3</f>
         <v>177120000</v>
       </c>
+      <c r="K3" s="2">
+        <f>SUMIFS(Table1[Chi],Table1[Phân loại],"Thiết bị") + SUMIFS(Table1[Chi],Table1[Phân loại],"Mặt bằng")</f>
+        <v>135369625</v>
+      </c>
       <c r="L3" s="2">
-        <f>SUMIFS(Table1[Chi],Table1[Phân loại],"Thiết bị") + SUMIFS(Table1[Chi],Table1[Phân loại],"Mặt bằng")</f>
-        <v>110841625</v>
-      </c>
-      <c r="M3" s="2">
-        <f>K3-L3</f>
-        <v>66278375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f>J3-K3</f>
+        <v>41750375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1383,22 +1419,23 @@
       <c r="G4" t="s">
         <v>188</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" t="s">
         <v>123</v>
       </c>
-      <c r="K4" s="2">
+      <c r="J4" s="2">
         <f>Budget!E4</f>
         <v>84000000</v>
       </c>
+      <c r="K4" s="2">
+        <f>SUMIFS(Table1[Chi],Table1[Phân loại],"Lương")</f>
+        <v>2500000</v>
+      </c>
       <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <f>K4-L4</f>
-        <v>84000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <f>J4-K4</f>
+        <v>81500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>101</v>
       </c>
@@ -1407,29 +1444,29 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
-        <v>3600000</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>190</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" t="s">
         <v>162</v>
       </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
       <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <f>SUM(Table1[Chi])-SUM(L2:L4)</f>
+        <f>SUM(Table1[Chi])-SUM(K2:K4)</f>
         <v>3948000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="21">
         <f>SUM(D2:D5)</f>
-        <v>193050000</v>
+        <v>213050000</v>
       </c>
       <c r="F6" s="2">
         <v>1500000</v>
@@ -1438,52 +1475,54 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>165</v>
       </c>
       <c r="D7" s="21">
         <f>SUM(D2:D5)+SUM(Table1[Thu])-SUM(Table1[Chi])</f>
-        <v>18760375</v>
+        <v>11732375</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <v>6000000</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>163</v>
       </c>
       <c r="D8" s="22">
         <f>D7-F9</f>
-        <v>4360375</v>
+        <v>9232375</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="2">
+        <v>500000</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="23" t="s">
         <v>164</v>
       </c>
       <c r="D9" s="24">
         <f>D8+E9</f>
-        <v>11310375</v>
+        <v>46182375</v>
       </c>
       <c r="E9" s="21">
         <f>SUM(E2:E5)</f>
-        <v>6950000</v>
+        <v>36950000</v>
       </c>
       <c r="F9" s="2">
         <f>SUM(F2:F8)</f>
-        <v>14400000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1505,11 +1544,11 @@
       <c r="G10" t="s">
         <v>4</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1532,7 +1571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ref="A12:A21" si="0">A11+1</f>
         <v>2</v>
@@ -1556,7 +1595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1580,7 +1619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1604,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1629,7 +1668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1800,7 +1839,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ref="A23:A57" si="1">A22+1</f>
+        <f t="shared" ref="A23:A72" si="1">A22+1</f>
         <v>13</v>
       </c>
       <c r="B23" s="1">
@@ -2040,7 +2079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -2064,7 +2103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2088,7 +2127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2112,7 +2151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2136,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -2160,7 +2199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2184,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2209,7 +2248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -2233,7 +2272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -2257,7 +2296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -2281,7 +2320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -2304,12 +2343,12 @@
       <c r="H43" t="s">
         <v>9</v>
       </c>
-      <c r="K43">
+      <c r="J43">
         <f>2.7+0.5+0.8+0.2+0.25+1</f>
         <v>5.45</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2333,7 +2372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2357,7 +2396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2381,7 +2420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2405,7 +2444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2626,55 +2665,330 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+      <c r="B57" s="1">
+        <v>42486</v>
+      </c>
+      <c r="D57" s="7">
+        <v>750000</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G57" t="s">
+        <v>193</v>
+      </c>
+      <c r="H57" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B58" s="1">
+        <v>42486</v>
+      </c>
+      <c r="D58" s="7">
+        <v>1500000</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G58" t="s">
+        <v>194</v>
+      </c>
+      <c r="H58" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B59" s="1">
+        <v>42486</v>
+      </c>
+      <c r="D59" s="7">
+        <v>1300000</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G59" t="s">
+        <v>192</v>
+      </c>
+      <c r="H59" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B60" s="1">
+        <v>42486</v>
+      </c>
+      <c r="D60" s="7">
+        <v>700000</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H60" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B61" s="1">
+        <v>42487</v>
+      </c>
+      <c r="D61" s="7">
+        <v>3600000</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G61" t="s">
+        <v>197</v>
+      </c>
+      <c r="H61" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B62" s="1">
+        <v>42487</v>
+      </c>
+      <c r="D62" s="7">
+        <v>9890000</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G62" t="s">
+        <v>199</v>
+      </c>
+      <c r="H62" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B63" s="1">
+        <v>42487</v>
+      </c>
+      <c r="D63" s="7">
+        <v>3990000</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G63" t="s">
+        <v>198</v>
+      </c>
+      <c r="H63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B64" s="1">
+        <v>42493</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G64" t="s">
+        <v>202</v>
+      </c>
+      <c r="H64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B65" s="1">
+        <v>42496</v>
+      </c>
+      <c r="D65" s="7">
+        <f>1200000+158000</f>
+        <v>1358000</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G65" t="s">
+        <v>203</v>
+      </c>
+      <c r="H65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B66" s="1">
+        <v>42496</v>
+      </c>
+      <c r="D66" s="7">
+        <v>1500000</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G66" t="s">
+        <v>204</v>
+      </c>
+      <c r="H66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B67" s="1">
+        <v>42497</v>
+      </c>
+      <c r="D67" s="7">
+        <v>1440000</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G67" t="s">
+        <v>188</v>
+      </c>
+      <c r="H67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B69" s="1"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>5</v>
       </c>
-      <c r="C63">
+      <c r="C73">
         <f>SUBTOTAL(109,Table1[Thu])</f>
         <v>0</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D73" s="4">
         <f>SUBTOTAL(109,Table1[Chi])</f>
-        <v>174289625</v>
-      </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
+        <v>201317625</v>
+      </c>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>